<commit_message>
TOR-57 Add handle multi die
* Refactor Dice class to support multiple dice rolls in 2d6
* Update configuration for reaction rolls
</commit_message>
<xml_diff>
--- a/data/Table.xlsx
+++ b/data/Table.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="407">
   <si>
     <t xml:space="preserve">die</t>
   </si>
@@ -1215,12 +1215,6 @@
     <t xml:space="preserve">Przywołać </t>
   </si>
   <si>
-    <t xml:space="preserve">roll1_d6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">roll2_d6</t>
-  </si>
-  <si>
     <t xml:space="preserve">2d6</t>
   </si>
   <si>
@@ -1230,10 +1224,19 @@
     <t xml:space="preserve">Hostile</t>
   </si>
   <si>
+    <t xml:space="preserve">[3,4,5]</t>
+  </si>
+  <si>
     <t xml:space="preserve">Unfriendly</t>
   </si>
   <si>
+    <t xml:space="preserve">[6,7,8]</t>
+  </si>
+  <si>
     <t xml:space="preserve">Unsure. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[9,10,11]</t>
   </si>
   <si>
     <t xml:space="preserve">Talkative. </t>
@@ -3638,10 +3641,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3653,515 +3656,45 @@
       <c r="B1" s="4" t="s">
         <v>398</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>399</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>400</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="B2" s="4" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>400</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="C3" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="D3" s="4" t="s">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
         <v>402</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>402</v>
+      <c r="B4" s="4" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="B5" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="C5" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>402</v>
+      <c r="A5" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="B6" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="C6" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B7" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B8" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="C8" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="B9" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="C9" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="B10" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="C10" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="B11" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C11" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="B12" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="C12" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="B13" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C13" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="B14" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="C14" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="B15" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="C15" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B16" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="C16" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="B17" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="C17" s="4" t="n">
-        <v>7</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="B18" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C18" s="4" t="n">
-        <v>7</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="B19" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="C19" s="4" t="n">
-        <v>7</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="B20" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="C20" s="4" t="n">
-        <v>7</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B21" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="C21" s="4" t="n">
-        <v>7</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="B22" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="C22" s="4" t="n">
-        <v>7</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="B23" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="C23" s="4" t="n">
-        <v>8</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="B24" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="C24" s="4" t="n">
-        <v>8</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B25" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="C25" s="4" t="n">
-        <v>8</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="B26" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="C26" s="4" t="n">
-        <v>8</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="B27" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="C27" s="4" t="n">
-        <v>8</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B28" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="C28" s="4" t="n">
-        <v>9</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="B29" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="C29" s="4" t="n">
-        <v>9</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="B30" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="C30" s="4" t="n">
-        <v>9</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="B31" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="C31" s="4" t="n">
-        <v>9</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="B32" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="C32" s="4" t="n">
-        <v>10</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="B33" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="C33" s="4" t="n">
-        <v>10</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="B34" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="C34" s="4" t="n">
-        <v>10</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="B35" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="C35" s="4" t="n">
-        <v>11</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="B36" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="C36" s="4" t="n">
-        <v>11</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="B37" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="C37" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="D37" s="4" t="s">
-        <v>405</v>
+      <c r="B6" s="4" t="s">
+        <v>406</v>
       </c>
     </row>
   </sheetData>

</xml_diff>